<commit_message>
Pushing the updates into the branch: release/1.0.1 sit
</commit_message>
<xml_diff>
--- a/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
+++ b/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
@@ -1180,7 +1180,7 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" t="b">
+      <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1245,7 +1245,7 @@
       <c r="F11" t="b">
         <v>0</v>
       </c>
-      <c r="G11" t="b">
+      <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="inlineStr">

</xml_diff>

<commit_message>
Pushing the updates into the branch: release/1.1.0 sit
</commit_message>
<xml_diff>
--- a/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
+++ b/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
@@ -1180,7 +1180,7 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" t="b">
+      <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1245,7 +1245,7 @@
       <c r="F11" t="b">
         <v>0</v>
       </c>
-      <c r="G11" t="b">
+      <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="inlineStr">

</xml_diff>

<commit_message>
Pushing the updates into the branch: release/1.0.3 sit
</commit_message>
<xml_diff>
--- a/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
+++ b/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
@@ -1302,7 +1302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1472,22 +1472,35 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>pull-sub-10</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>pull-sub-10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>topic-10</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>60</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2400s</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Pushing the updates into the branch: release/1.0.4 sit
</commit_message>
<xml_diff>
--- a/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
+++ b/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
@@ -1302,7 +1302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1502,6 +1502,37 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>pull-sub-11</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>pull-sub-11</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>topic-8</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>120</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2700s</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Pushing the updates into the branch: release/1.0.5 sit
</commit_message>
<xml_diff>
--- a/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
+++ b/helm-charts/sit-values/infra-values/dataset/infra_sheet.xlsx
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1503,35 +1503,13 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>pull-sub-11</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>pull-sub-11</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>topic-8</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>120</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2700s</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>6</v>
-      </c>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>